<commit_message>
re for date is fixed
</commit_message>
<xml_diff>
--- a/testpdf/example.xlsx
+++ b/testpdf/example.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\mypy\PDFConv2\testpdf\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
   <si>
     <t>Дата договора</t>
   </si>
@@ -25,33 +30,14 @@
     <t>14 декабря 2022</t>
   </si>
   <si>
-    <t>Not Found</t>
-  </si>
-  <si>
-    <t>16
-ИНН 7736</t>
-  </si>
-  <si>
-    <t>14декабря 2022</t>
-  </si>
-  <si>
-    <t>16,номер 9140</t>
-  </si>
-  <si>
-    <t>25.05.2017</t>
-  </si>
-  <si>
-    <t>14.12.2022</t>
-  </si>
-  <si>
     <t>348/2022/94</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -110,17 +96,25 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -158,9 +152,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -192,9 +186,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -226,9 +221,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -401,14 +397,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B32"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -416,251 +414,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" t="s">
-        <v>6</v>
-      </c>
-      <c r="B13" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" t="s">
-        <v>6</v>
-      </c>
-      <c r="B14" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15" t="s">
-        <v>6</v>
-      </c>
-      <c r="B15" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" t="s">
-        <v>6</v>
-      </c>
-      <c r="B16" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" t="s">
-        <v>6</v>
-      </c>
-      <c r="B17" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" t="s">
-        <v>6</v>
-      </c>
-      <c r="B18" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" t="s">
-        <v>6</v>
-      </c>
-      <c r="B19" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" t="s">
-        <v>7</v>
-      </c>
-      <c r="B20" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" t="s">
-        <v>6</v>
-      </c>
-      <c r="B21" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22" t="s">
-        <v>6</v>
-      </c>
-      <c r="B22" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="A23" t="s">
-        <v>6</v>
-      </c>
-      <c r="B23" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="A24" t="s">
-        <v>6</v>
-      </c>
-      <c r="B24" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2">
-      <c r="A25" t="s">
-        <v>6</v>
-      </c>
-      <c r="B25" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2">
-      <c r="A26" t="s">
-        <v>6</v>
-      </c>
-      <c r="B26" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2">
-      <c r="A27" t="s">
-        <v>6</v>
-      </c>
-      <c r="B27" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2">
-      <c r="A28" t="s">
-        <v>3</v>
-      </c>
-      <c r="B28" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2">
-      <c r="A29" t="s">
-        <v>8</v>
-      </c>
-      <c r="B29" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2">
-      <c r="A30" t="s">
-        <v>8</v>
-      </c>
-      <c r="B30" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2">
-      <c r="A31" t="s">
-        <v>3</v>
-      </c>
-      <c r="B31" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2">
-      <c r="A32" t="s">
-        <v>3</v>
-      </c>
-      <c r="B32" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>